<commit_message>
담당 manager 정보 report 에 적용
</commit_message>
<xml_diff>
--- a/gluonkorea_report/public/xlsxTemplate/11stSellerTemplate.xlsx
+++ b/gluonkorea_report/public/xlsxTemplate/11stSellerTemplate.xlsx
@@ -200,14 +200,6 @@
     <phoneticPr fontId="39" type="noConversion"/>
   </si>
   <si>
-    <t>ROAS</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>ROAS</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="39" type="noConversion"/>
   </si>
@@ -266,6 +258,14 @@
   <si>
     <t>◇ 광고영역별 요약</t>
     <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROI</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROI</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -14088,6 +14088,21 @@
     <xf numFmtId="178" fontId="10" fillId="34" borderId="29" xfId="4011" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="181" fontId="11" fillId="34" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="11" fillId="34" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -14152,21 +14167,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="43" xfId="4100" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="181" fontId="11" fillId="34" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="11" fillId="34" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -18518,8 +18518,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1545807936"/>
-        <c:axId val="-1545805456"/>
+        <c:axId val="-1549831408"/>
+        <c:axId val="-1620145552"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -18533,7 +18533,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ROAS</c:v>
+                  <c:v>ROI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -18609,11 +18609,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1545800496"/>
-        <c:axId val="-1545802976"/>
+        <c:axId val="-1592271584"/>
+        <c:axId val="-1592273904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1545807936"/>
+        <c:axId val="-1549831408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18623,7 +18623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1545805456"/>
+        <c:crossAx val="-1620145552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18631,7 +18631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1545805456"/>
+        <c:axId val="-1620145552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18641,12 +18641,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1545807936"/>
+        <c:crossAx val="-1549831408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1545802976"/>
+        <c:axId val="-1592273904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18656,12 +18656,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1545800496"/>
+        <c:crossAx val="-1592271584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1545800496"/>
+        <c:axId val="-1592271584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18671,7 +18671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="-1545802976"/>
+        <c:crossAx val="-1592273904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18834,8 +18834,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1587764304"/>
-        <c:axId val="-1587761744"/>
+        <c:axId val="-1588357120"/>
+        <c:axId val="-1591996960"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -18849,7 +18849,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ROAS</c:v>
+                  <c:v>ROI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -18894,11 +18894,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1591767376"/>
-        <c:axId val="-1591769696"/>
+        <c:axId val="-1591992320"/>
+        <c:axId val="-1591994640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1587764304"/>
+        <c:axId val="-1588357120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18908,7 +18908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1587761744"/>
+        <c:crossAx val="-1591996960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18916,7 +18916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1587761744"/>
+        <c:axId val="-1591996960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18926,12 +18926,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1587764304"/>
+        <c:crossAx val="-1588357120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1591769696"/>
+        <c:axId val="-1591994640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18941,12 +18941,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1591767376"/>
+        <c:crossAx val="-1591992320"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1591767376"/>
+        <c:axId val="-1591992320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18956,7 +18956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="-1591769696"/>
+        <c:crossAx val="-1591994640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19408,11 +19408,11 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" ht="36" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -19433,70 +19433,70 @@
       <c r="B4" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="105"/>
+      <c r="D4" s="110"/>
       <c r="E4" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="108" t="s">
+      <c r="F4" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="109"/>
-      <c r="H4" s="110"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="115"/>
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="102" t="s">
-        <v>46</v>
+      <c r="C5" s="107" t="s">
+        <v>44</v>
       </c>
-      <c r="D5" s="103"/>
+      <c r="D5" s="108"/>
       <c r="E5" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="111" t="s">
+      <c r="F5" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="112"/>
-      <c r="H5" s="113"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="118"/>
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="102" t="s">
-        <v>47</v>
+      <c r="C6" s="107" t="s">
+        <v>45</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="98" t="s">
+      <c r="D6" s="108"/>
+      <c r="E6" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="111" t="s">
+      <c r="F6" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="113"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="118"/>
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="107"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="95" t="s">
+      <c r="D7" s="112"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="96"/>
-      <c r="H7" s="97"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="102"/>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -19505,10 +19505,10 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="114"/>
+      <c r="C9" s="92"/>
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -19530,7 +19530,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="85" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="G11" s="68"/>
       <c r="H11" s="15"/>
@@ -19538,7 +19538,7 @@
     <row r="12" spans="1:9" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="71" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="34">
         <v>96008</v>
@@ -19559,7 +19559,7 @@
     <row r="13" spans="1:9" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="72" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="36">
         <v>83831</v>
@@ -19627,24 +19627,24 @@
     </row>
     <row r="16" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
-      <c r="B16" s="101" t="s">
+      <c r="B16" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
@@ -19826,10 +19826,10 @@
     </row>
     <row r="34" spans="1:9" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="114" t="s">
-        <v>55</v>
+      <c r="B34" s="92" t="s">
+        <v>53</v>
       </c>
-      <c r="C34" s="114"/>
+      <c r="C34" s="92"/>
       <c r="D34" s="7"/>
       <c r="E34" s="26"/>
       <c r="G34" s="6"/>
@@ -19839,12 +19839,12 @@
     <row r="35" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:9" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="79" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
-      <c r="C36" s="93" t="s">
+      <c r="C36" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="94"/>
+      <c r="D36" s="99"/>
       <c r="E36" s="80" t="s">
         <v>7</v>
       </c>
@@ -19863,13 +19863,13 @@
     </row>
     <row r="37" spans="1:9" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
-      <c r="B37" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="115" t="s">
+      <c r="B37" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="116"/>
+      <c r="C37" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="94"/>
       <c r="E37" s="76"/>
       <c r="F37" s="76"/>
       <c r="G37" s="76"/>
@@ -19881,11 +19881,11 @@
     </row>
     <row r="38" spans="1:9" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
-      <c r="B38" s="118"/>
-      <c r="C38" s="115" t="s">
-        <v>52</v>
+      <c r="B38" s="96"/>
+      <c r="C38" s="93" t="s">
+        <v>50</v>
       </c>
-      <c r="D38" s="116"/>
+      <c r="D38" s="94"/>
       <c r="E38" s="78"/>
       <c r="F38" s="78"/>
       <c r="G38" s="78"/>
@@ -19897,10 +19897,10 @@
     </row>
     <row r="39" spans="1:9" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
-      <c r="B39" s="92" t="s">
-        <v>50</v>
+      <c r="B39" s="97" t="s">
+        <v>48</v>
       </c>
-      <c r="C39" s="92"/>
+      <c r="C39" s="97"/>
       <c r="D39" s="75">
         <f>C60</f>
         <v>0</v>
@@ -19939,10 +19939,10 @@
     </row>
     <row r="41" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
-      <c r="B41" s="114" t="s">
+      <c r="B41" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="114"/>
+      <c r="C41" s="92"/>
       <c r="D41" s="7"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -20128,10 +20128,10 @@
     </row>
     <row r="58" spans="1:9" s="11" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
-      <c r="B58" s="114" t="s">
+      <c r="B58" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="114"/>
+      <c r="C58" s="92"/>
       <c r="D58" s="7"/>
       <c r="E58" s="26"/>
       <c r="G58" s="6"/>
@@ -20167,7 +20167,7 @@
     <row r="60" spans="1:9" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C60" s="63">
         <f>SUM(C61:C67)</f>
@@ -20335,7 +20335,7 @@
     <row r="72" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
       <c r="B72" s="44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C72" s="45"/>
       <c r="D72" s="45"/>
@@ -20348,7 +20348,7 @@
     <row r="73" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
       <c r="B73" s="46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
@@ -20361,7 +20361,7 @@
     <row r="74" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
       <c r="B74" s="46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -20373,7 +20373,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B75" s="58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
@@ -20385,7 +20385,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B76" s="46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
@@ -20397,7 +20397,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B77" s="46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
@@ -20410,7 +20410,7 @@
     <row r="78" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9"/>
       <c r="B78" s="58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
@@ -20423,7 +20423,7 @@
     <row r="79" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9"/>
       <c r="B79" s="58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
@@ -20436,7 +20436,7 @@
     <row r="80" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9"/>
       <c r="B80" s="46" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
@@ -20449,7 +20449,7 @@
     <row r="81" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
       <c r="B81" s="58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
@@ -20462,7 +20462,7 @@
     <row r="82" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
       <c r="B82" s="58" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
@@ -20475,7 +20475,7 @@
     <row r="83" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="9"/>
       <c r="B83" s="59" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C83" s="48"/>
       <c r="D83" s="48"/>
@@ -20505,14 +20505,8 @@
     <sortCondition descending="1" ref="F36:F140"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="B2:D2"/>
@@ -20525,8 +20519,14 @@
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="F6:H6"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.23622047244094491" bottom="0.27559055118110237" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -20564,7 +20564,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>